<commit_message>
chore(data): update sample laptop dataset
</commit_message>
<xml_diff>
--- a/src/app/examples/dataset-laptop.xlsx
+++ b/src/app/examples/dataset-laptop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 5 Data Mining\ProjectUAS-Data-Mining\src\app\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0073AB2-949A-4BFE-9EF5-DDBE2645627C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D391E1F7-4E98-4D0F-B523-E26C422DCBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="750" windowWidth="20730" windowHeight="10890" xr2:uid="{76B7460A-A3BE-4490-95B4-A6943895C009}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -144,25 +144,28 @@
     <t>G 15</t>
   </si>
   <si>
-    <t>rtx3050</t>
-  </si>
-  <si>
     <t>Aspire Lite 15 (AL15-42P)</t>
   </si>
   <si>
     <t>Integrated Graphics</t>
   </si>
   <si>
-    <t>AMD Ryzen 5 7430U</t>
-  </si>
-  <si>
-    <t>512 SSD NVME</t>
-  </si>
-  <si>
-    <t>15.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 GB DDR4 SDRAM </t>
+    <t>NVIDIA GeForce RTX 3050</t>
+  </si>
+  <si>
+    <t>Apple M1 GPU</t>
+  </si>
+  <si>
+    <t>NVIDIA GeForce RTX 4050</t>
+  </si>
+  <si>
+    <t>Intel Iris Xe Graphics</t>
+  </si>
+  <si>
+    <t>NVIDIA GeForce RTX 4060</t>
+  </si>
+  <si>
+    <t>NVIDIA GeForce RTX 4070</t>
   </si>
 </sst>
 </file>
@@ -518,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0D241A-FBA5-4488-8A6A-5926FF839D76}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +533,7 @@
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -575,22 +578,22 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>7900</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>512</v>
+      </c>
+      <c r="G2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>41</v>
+      <c r="H2" s="1">
+        <v>15</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -615,14 +618,17 @@
       <c r="E3">
         <v>16</v>
       </c>
+      <c r="F3">
+        <v>512</v>
+      </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H3">
         <v>15</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>6800000</v>
@@ -644,14 +650,17 @@
       <c r="E4">
         <v>8</v>
       </c>
+      <c r="F4">
+        <v>512</v>
+      </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>7000000</v>
@@ -670,14 +679,20 @@
       <c r="D5">
         <v>3000</v>
       </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>512</v>
+      </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I5">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>9000000</v>
@@ -696,14 +711,20 @@
       <c r="D6">
         <v>6200</v>
       </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>512</v>
+      </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H6">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <v>8500000</v>
@@ -722,17 +743,23 @@
       <c r="D7">
         <v>12000</v>
       </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>256</v>
+      </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H7">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I7">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>7600000</v>
+        <v>14500000</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -748,17 +775,23 @@
       <c r="D8">
         <v>9000</v>
       </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>512</v>
+      </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>12500000</v>
+        <v>15500000</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -774,17 +807,23 @@
       <c r="D9">
         <v>7500</v>
       </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>512</v>
+      </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H9">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I9">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>9000000</v>
+        <v>12500000</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -800,17 +839,23 @@
       <c r="D10">
         <v>6800</v>
       </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>512</v>
+      </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H10">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I10">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>8800000</v>
+        <v>11800000</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -826,17 +871,23 @@
       <c r="D11">
         <v>8000</v>
       </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>512</v>
+      </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H11">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I11">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>18000000</v>
+        <v>13200000</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -852,17 +903,23 @@
       <c r="D12">
         <v>11500</v>
       </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>512</v>
+      </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H12">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I12">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>9000000</v>
+        <v>19000000</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -878,17 +935,23 @@
       <c r="D13">
         <v>8800</v>
       </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>512</v>
+      </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H13">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I13">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="J13">
-        <v>8000000</v>
+        <v>13000000</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -904,17 +967,23 @@
       <c r="D14">
         <v>9500</v>
       </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>512</v>
+      </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H14">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I14">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <v>12000000</v>
+        <v>17000000</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -930,17 +999,23 @@
       <c r="D15">
         <v>10500</v>
       </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>512</v>
+      </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H15">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I15">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>13000000</v>
+        <v>18500000</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -956,17 +1031,23 @@
       <c r="D16">
         <v>9800</v>
       </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>512</v>
+      </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H16">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I16">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>14000000</v>
+        <v>16500000</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,17 +1063,23 @@
       <c r="D17">
         <v>11000</v>
       </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>512</v>
+      </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H17">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="I17">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="J17">
-        <v>16000000</v>
+        <v>23000000</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1008,17 +1095,23 @@
       <c r="D18">
         <v>9200</v>
       </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>512</v>
+      </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H18">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I18">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="J18">
-        <v>15000000</v>
+        <v>19500000</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1034,17 +1127,23 @@
       <c r="D19">
         <v>7000</v>
       </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>1024</v>
+      </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H19">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="I19">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>17000000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,17 +1159,23 @@
       <c r="D20">
         <v>14000</v>
       </c>
+      <c r="E20">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>1024</v>
+      </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H20">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="I20">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="J20">
-        <v>14000000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1085,6 +1190,24 @@
       </c>
       <c r="D21">
         <v>12500</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>1024</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21">
+        <v>15</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>24000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>